<commit_message>
Fixed transmittal issue in which values would be placed in cells according to their number and not the correct table row
</commit_message>
<xml_diff>
--- a/Templates/Stamp.xlsx
+++ b/Templates/Stamp.xlsx
@@ -193,6 +193,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -201,9 +204,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,7 +488,7 @@
   <dimension ref="A9:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,34 +539,34 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="14"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="9"/>
       <c r="D19" s="7"/>
       <c r="E19" s="6"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="9"/>
       <c r="D20" s="7"/>
       <c r="E20" s="6"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="9"/>
       <c r="D21" s="7"/>
       <c r="E21" s="6"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="9"/>
       <c r="D22" s="7"/>
       <c r="E22" s="6"/>
@@ -605,82 +605,82 @@
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="15"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -706,7 +706,7 @@
       </c>
       <c r="B45" s="8">
         <f ca="1">TODAY()</f>
-        <v>42594</v>
+        <v>42544</v>
       </c>
     </row>
   </sheetData>

</xml_diff>